<commit_message>
Began writing parser in python. changed player CSV file
</commit_message>
<xml_diff>
--- a/excel documents/player.xlsx
+++ b/excel documents/player.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\github\1dv503\database_assignment3\excel documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/775cb088da073b9b/Dokument/Knacka_kod/Phyton/1DV503/database_assignment3/excel documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33839F2F-9228-4A04-BF60-77BFA137AA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{33839F2F-9228-4A04-BF60-77BFA137AA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27292E7B-C897-42C1-9CB2-0A11690713E6}"/>
   <bookViews>
-    <workbookView xWindow="4845" yWindow="1530" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2712" yWindow="2112" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
@@ -39,9 +39,6 @@
     <t>nationality</t>
   </si>
   <si>
-    <t>discs</t>
-  </si>
-  <si>
     <t>Alex Smith</t>
   </si>
   <si>
@@ -51,18 +48,12 @@
     <t>USA</t>
   </si>
   <si>
-    <t>river,keystone,pure,explorer</t>
-  </si>
-  <si>
     <t>John glenn</t>
   </si>
   <si>
     <t>pro</t>
   </si>
   <si>
-    <t>knigth,cutlass,compass,pain</t>
-  </si>
-  <si>
     <t>Mia venetto</t>
   </si>
   <si>
@@ -72,43 +63,19 @@
     <t>Italy</t>
   </si>
   <si>
-    <t>Explorer,River, pure,gauntlet,fuse</t>
-  </si>
-  <si>
     <t>Daniel Ekstrom</t>
   </si>
   <si>
     <t>Sweden</t>
   </si>
   <si>
-    <t>river,compass,fuse,explorer,cutlass,knigth,gauntlet,keystone,pure,pain</t>
-  </si>
-  <si>
     <t>Johan Gustafsson</t>
   </si>
   <si>
-    <t>sweden</t>
-  </si>
-  <si>
-    <t>river,compass,keystone</t>
-  </si>
-  <si>
     <t>Max Pettersson</t>
   </si>
   <si>
-    <t>ádvanced</t>
-  </si>
-  <si>
-    <t>river,compass,cutlass,pure</t>
-  </si>
-  <si>
     <t>Linus Carlsson</t>
-  </si>
-  <si>
-    <t>Pro</t>
-  </si>
-  <si>
-    <t>swedden</t>
   </si>
 </sst>
 </file>
@@ -426,18 +393,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H15:H16"/>
+      <selection activeCell="E1" sqref="E1:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,127 +417,103 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1001</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1002</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1003</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1004</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1005</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1006</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1007</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>